<commit_message>
Idk co všechno jsem udělal
</commit_message>
<xml_diff>
--- a/results_xlsx/prednasky_bez_prednasejicich.xlsx
+++ b/results_xlsx/prednasky_bez_prednasejicich.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="252">
   <si>
     <t>katedra</t>
   </si>
@@ -70,12 +70,12 @@
     <t>KGEO</t>
   </si>
   <si>
+    <t>KBI</t>
+  </si>
+  <si>
     <t>KFY</t>
   </si>
   <si>
-    <t>KBI</t>
-  </si>
-  <si>
     <t>CNB</t>
   </si>
   <si>
@@ -91,9 +91,6 @@
     <t>B107</t>
   </si>
   <si>
-    <t>B200</t>
-  </si>
-  <si>
     <t>B203</t>
   </si>
   <si>
@@ -112,6 +109,18 @@
     <t>BK100</t>
   </si>
   <si>
+    <t>BK201</t>
+  </si>
+  <si>
+    <t>BK333</t>
+  </si>
+  <si>
+    <t>BP201</t>
+  </si>
+  <si>
+    <t>BP333</t>
+  </si>
+  <si>
     <t>FORT</t>
   </si>
   <si>
@@ -124,12 +133,18 @@
     <t>KMECH</t>
   </si>
   <si>
-    <t>KN323</t>
+    <t>KN102</t>
   </si>
   <si>
     <t>M100</t>
   </si>
   <si>
+    <t>M102</t>
+  </si>
+  <si>
+    <t>M104</t>
+  </si>
+  <si>
     <t>M105</t>
   </si>
   <si>
@@ -148,10 +163,13 @@
     <t>M316</t>
   </si>
   <si>
+    <t>MA100</t>
+  </si>
+  <si>
     <t>MECH</t>
   </si>
   <si>
-    <t>N323</t>
+    <t>N102</t>
   </si>
   <si>
     <t>NA01</t>
@@ -163,6 +181,18 @@
     <t>NA06</t>
   </si>
   <si>
+    <t>OCHE</t>
+  </si>
+  <si>
+    <t>P102</t>
+  </si>
+  <si>
+    <t>P201</t>
+  </si>
+  <si>
+    <t>P391</t>
+  </si>
+  <si>
     <t>PB333</t>
   </si>
   <si>
@@ -181,12 +211,12 @@
     <t>1.10.2024</t>
   </si>
   <si>
+    <t>19.2.2025</t>
+  </si>
+  <si>
     <t>2.10.2024</t>
   </si>
   <si>
-    <t>19.2.2025</t>
-  </si>
-  <si>
     <t>4.10.2024</t>
   </si>
   <si>
@@ -196,22 +226,25 @@
     <t>8.11.2024</t>
   </si>
   <si>
+    <t>16.11.2024</t>
+  </si>
+  <si>
     <t>26.10.2024</t>
   </si>
   <si>
     <t>5.10.2024</t>
   </si>
   <si>
+    <t>19.10.2024</t>
+  </si>
+  <si>
     <t>1.11.2024</t>
   </si>
   <si>
-    <t>19.10.2024</t>
-  </si>
-  <si>
-    <t>20.12.2024</t>
-  </si>
-  <si>
-    <t>13.12.2024</t>
+    <t>14.12.2024</t>
+  </si>
+  <si>
+    <t>30.11.2024</t>
   </si>
   <si>
     <t>3.10.2024</t>
@@ -223,12 +256,12 @@
     <t>17.12.2024</t>
   </si>
   <si>
+    <t>14.5.2025</t>
+  </si>
+  <si>
     <t>18.12.2024</t>
   </si>
   <si>
-    <t>14.5.2025</t>
-  </si>
-  <si>
     <t>3.1.2025</t>
   </si>
   <si>
@@ -247,24 +280,24 @@
     <t>14:00</t>
   </si>
   <si>
+    <t>17:00</t>
+  </si>
+  <si>
+    <t>12:00</t>
+  </si>
+  <si>
+    <t>11:00</t>
+  </si>
+  <si>
+    <t>10:00</t>
+  </si>
+  <si>
+    <t>09:00</t>
+  </si>
+  <si>
     <t>08:00</t>
   </si>
   <si>
-    <t>09:00</t>
-  </si>
-  <si>
-    <t>17:00</t>
-  </si>
-  <si>
-    <t>12:00</t>
-  </si>
-  <si>
-    <t>11:00</t>
-  </si>
-  <si>
-    <t>10:00</t>
-  </si>
-  <si>
     <t>17:50</t>
   </si>
   <si>
@@ -277,27 +310,30 @@
     <t>15:50</t>
   </si>
   <si>
+    <t>18:50</t>
+  </si>
+  <si>
+    <t>13:50</t>
+  </si>
+  <si>
+    <t>11:50</t>
+  </si>
+  <si>
+    <t>12:50</t>
+  </si>
+  <si>
+    <t>19:50</t>
+  </si>
+  <si>
+    <t>10:50</t>
+  </si>
+  <si>
+    <t>20:50</t>
+  </si>
+  <si>
     <t>09:50</t>
   </si>
   <si>
-    <t>10:50</t>
-  </si>
-  <si>
-    <t>18:50</t>
-  </si>
-  <si>
-    <t>13:50</t>
-  </si>
-  <si>
-    <t>11:50</t>
-  </si>
-  <si>
-    <t>12:50</t>
-  </si>
-  <si>
-    <t>19:50</t>
-  </si>
-  <si>
     <t>101KPRF</t>
   </si>
   <si>
@@ -310,9 +346,6 @@
     <t>B107KGEO</t>
   </si>
   <si>
-    <t>B200KCH</t>
-  </si>
-  <si>
     <t>B203KGEO</t>
   </si>
   <si>
@@ -331,6 +364,18 @@
     <t>BK100KCH</t>
   </si>
   <si>
+    <t>BK201KBI</t>
+  </si>
+  <si>
+    <t>BK333KBI</t>
+  </si>
+  <si>
+    <t>BP201KBI</t>
+  </si>
+  <si>
+    <t>BP333KBI</t>
+  </si>
+  <si>
     <t>FORTKFY</t>
   </si>
   <si>
@@ -343,13 +388,16 @@
     <t>KMECHKFY</t>
   </si>
   <si>
-    <t>KN323KCH</t>
+    <t>KN102KBI</t>
   </si>
   <si>
     <t>M100KCH</t>
   </si>
   <si>
-    <t>M100CNB</t>
+    <t>M102KBI</t>
+  </si>
+  <si>
+    <t>M104KCH</t>
   </si>
   <si>
     <t>M105KGEO</t>
@@ -370,10 +418,13 @@
     <t>M316KGEO</t>
   </si>
   <si>
+    <t>MA100KBI</t>
+  </si>
+  <si>
     <t>MECHKFY</t>
   </si>
   <si>
-    <t>N323KCH</t>
+    <t>N102KBI</t>
   </si>
   <si>
     <t>NA01KFY</t>
@@ -385,6 +436,18 @@
     <t>NA06CNB</t>
   </si>
   <si>
+    <t>OCHEKCH</t>
+  </si>
+  <si>
+    <t>P102KBI</t>
+  </si>
+  <si>
+    <t>P201KBI</t>
+  </si>
+  <si>
+    <t>P391KCH</t>
+  </si>
+  <si>
     <t>PB333KBI</t>
   </si>
   <si>
@@ -403,9 +466,6 @@
     <t>Fyzická geografie I</t>
   </si>
   <si>
-    <t>Organická chemie</t>
-  </si>
-  <si>
     <t>Geografie Česka I</t>
   </si>
   <si>
@@ -421,22 +481,26 @@
     <t>Ochrana přírody a krajiny</t>
   </si>
   <si>
+    <t>Chemie a fyzika živých soustav</t>
+  </si>
+  <si>
+    <t>Biologie prokaryot a virů</t>
+  </si>
+  <si>
     <t>Programování - Fortran</t>
   </si>
   <si>
-    <t>Biologie prokaryot a virů</t>
-  </si>
-  <si>
     <t>Mechanika</t>
   </si>
   <si>
-    <t>Organická chemie Nmgr.</t>
+    <t>Biologie členovců</t>
   </si>
   <si>
     <t>Fyzikální chemie NMgr.</t>
   </si>
   <si>
-    <t>Vědecká komunikace v biologii</t>
+    <t xml:space="preserve">Metody charakterizace látek a materiálů
+</t>
   </si>
   <si>
     <t>Didaktika geografie I</t>
@@ -457,6 +521,9 @@
     <t>Fyzická geografie Evropy</t>
   </si>
   <si>
+    <t>Vybrané kapitoly z etologie bezobratlých</t>
+  </si>
+  <si>
     <t>Úvod do kvantové fyziky a spektroskopie</t>
   </si>
   <si>
@@ -466,6 +533,12 @@
     <t>Struk. látek a difr. analýza v mat. výz.</t>
   </si>
   <si>
+    <t>Obecná chemie</t>
+  </si>
+  <si>
+    <t>Úvod do studia biologie</t>
+  </si>
+  <si>
     <t>Úvod do počítačového modelování</t>
   </si>
   <si>
@@ -481,16 +554,13 @@
     <t>'RNDr. Ivan Farský, CSc.', 'Mgr. Jiří Riezner, Ph.D.'</t>
   </si>
   <si>
-    <t>'doc. Ing. Jan Čermák, CSc.'</t>
-  </si>
-  <si>
     <t>'doc. Mgr. Pavel Raška, Ph.D.'</t>
   </si>
   <si>
     <t>'Mgr. Vladan Hruška, Ph.D.'</t>
   </si>
   <si>
-    <t>'doc. Ing. Jan Čermák, CSc.', 'RNDr. Thu Huong Nguyen Thi, Ph.D.'</t>
+    <t>'RNDr. Thu Huong Nguyen Thi, Ph.D.'</t>
   </si>
   <si>
     <t>'doc. RNDr. Jiří Anděl, CSc.'</t>
@@ -499,6 +569,9 @@
     <t>'RNDr. Tomáš Matějček, Ph.D.'</t>
   </si>
   <si>
+    <t>'RNDr. Jan Ipser, CSc.'</t>
+  </si>
+  <si>
     <t>'Mgr. Martin Svoboda, Ph.D.'</t>
   </si>
   <si>
@@ -508,10 +581,13 @@
     <t>'RNDr. Martin Švec, Ph.D.'</t>
   </si>
   <si>
+    <t>'Mgr. Michaela Czerneková, Ph.D.', 'doc. RNDr. Jaromír Hajer, CSc.', 'Mgr. Michal Holec, Ph.D.'</t>
+  </si>
+  <si>
     <t>'prof. Ing. Zdeňka Kolská, Ph.D.'</t>
   </si>
   <si>
-    <t>'doc. RNDr. Jaromír Hajer, CSc.', 'doc. RNDr. Eva Jozífková, Ph.D. et Ph.D.', 'Mgr. Jan Malý, Ph.D.'</t>
+    <t>'doc. Ing. Jiří Henych, Ph.D.', 'prof. Ing. Zdeňka Kolská, Ph.D.', 'RNDr. Petr Ryšánek, Ph.D.', 'RNDr. Václav Šícha, Ph.D.', 'Ing. Magda Škvorová, Ph.D.', 'Mgr. Marcel Štofik, Ph.D.', 'Ing. Jitka Tolaszová, Ph.D.', 'RNDr. Ľuboš Vrtoch, Ph.D.'</t>
   </si>
   <si>
     <t>'RNDr. Silvie Rita Kučerová, Ph.D.'</t>
@@ -526,6 +602,9 @@
     <t>'Mgr. Jiří Riezner, Ph.D.'</t>
   </si>
   <si>
+    <t>'Mgr. Michaela Czerneková, Ph.D.', 'doc. RNDr. Jaromír Hajer, CSc.'</t>
+  </si>
+  <si>
     <t>'prof. Ing. Zdeňka Kolská, Ph.D.', 'doc. Ing. Martin Kormunda, Ph.D.', 'Mgr. Jan Malý, Ph.D.'</t>
   </si>
   <si>
@@ -547,16 +626,13 @@
     <t>315, 3164</t>
   </si>
   <si>
-    <t>1064</t>
-  </si>
-  <si>
     <t>1434</t>
   </si>
   <si>
     <t>4222</t>
   </si>
   <si>
-    <t>1064, 429</t>
+    <t>429</t>
   </si>
   <si>
     <t>312</t>
@@ -565,6 +641,9 @@
     <t>1472</t>
   </si>
   <si>
+    <t>930</t>
+  </si>
+  <si>
     <t>5958</t>
   </si>
   <si>
@@ -574,10 +653,13 @@
     <t>613</t>
   </si>
   <si>
+    <t>8018, 278, 555</t>
+  </si>
+  <si>
     <t>332</t>
   </si>
   <si>
-    <t>278, 2939, 280</t>
+    <t>5431, 332, 4587, 4310, 2856, 1503, 5135, 4117</t>
   </si>
   <si>
     <t>3528</t>
@@ -592,6 +674,9 @@
     <t>3164</t>
   </si>
   <si>
+    <t>8018, 278</t>
+  </si>
+  <si>
     <t>332, 2384, 280</t>
   </si>
   <si>
@@ -619,9 +704,6 @@
     <t>Vágner Jiří, RNDr. Ph.D.</t>
   </si>
   <si>
-    <t>Babor Martin, Ing. Ph.D.</t>
-  </si>
-  <si>
     <t>Riezner Jiří, Mgr. Ph.D.</t>
   </si>
   <si>
@@ -634,22 +716,31 @@
     <t>Martínek Jiří, RNDr. Ph.D.</t>
   </si>
   <si>
+    <t>Benada Oldřich, RNDr. CSc.</t>
+  </si>
+  <si>
+    <t>Šebestová Janoušková Olga, Mgr. Ph.D.</t>
+  </si>
+  <si>
     <t>Moučka Filip, doc. RNDr. Ph.D.</t>
   </si>
   <si>
-    <t>Šebestová Janoušková Olga, Mgr. Ph.D.</t>
-  </si>
-  <si>
     <t>Dočkal Jan, RNDr. Ph.D.</t>
   </si>
   <si>
+    <t>Klečka Jan, RNDr. Ph.D.</t>
+  </si>
+  <si>
+    <t>Jirsák Jan, doc. RNDr. Ph.D.</t>
+  </si>
+  <si>
     <t>Škvorová Magda, Ing. Ph.D.</t>
   </si>
   <si>
-    <t>Jirsák Jan, doc. RNDr. Ph.D.</t>
-  </si>
-  <si>
-    <t>Gryndler Milan, prof. doc. RNDr. CSc.</t>
+    <t>Kaule Pavel, Mgr.</t>
+  </si>
+  <si>
+    <t>Greguš Viktor, Ing.</t>
   </si>
   <si>
     <t>Trahorsch Petr, Mgr. Ph.D.</t>
@@ -674,6 +765,9 @@
   </si>
   <si>
     <t>Daniš Stanislav, doc. RNDr. Ph.D.</t>
+  </si>
+  <si>
+    <t>Herma Regina, RNDr. Ph.D.</t>
   </si>
   <si>
     <t>Čapková Pavla, prof. RNDr. DrSc.</t>
@@ -738,8 +832,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Frame0" displayName="Frame0" ref="A1:O40" totalsRowShown="0">
-  <autoFilter ref="A1:O40"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Frame0" displayName="Frame0" ref="A1:O50" totalsRowShown="0">
+  <autoFilter ref="A1:O50"/>
   <tableColumns count="15">
     <tableColumn id="1" name="katedra" dataDxfId="0"/>
     <tableColumn id="2" name="zkratka" dataDxfId="0"/>
@@ -1046,7 +1140,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O40"/>
+  <dimension ref="A1:O50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1110,32 +1204,32 @@
         <v>556</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E2" s="2">
         <v>2024</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1" t="s">
-        <v>196</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -1149,40 +1243,40 @@
         <v>3705</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E3" s="2">
         <v>2024</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>126</v>
+        <v>147</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>152</v>
+        <v>176</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>174</v>
+        <v>200</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>197</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -1196,40 +1290,40 @@
         <v>4303</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E4" s="2">
         <v>2024</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>127</v>
+        <v>148</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>153</v>
+        <v>177</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>175</v>
+        <v>201</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>198</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -1243,40 +1337,40 @@
         <v>5855</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E5" s="2">
         <v>2024</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>17</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>127</v>
+        <v>148</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>153</v>
+        <v>177</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>175</v>
+        <v>201</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>199</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -1290,181 +1384,181 @@
         <v>4398</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E6" s="2">
         <v>2024</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>17</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>128</v>
+        <v>149</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>154</v>
+        <v>178</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>176</v>
+        <v>202</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>200</v>
+        <v>228</v>
       </c>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C7" s="2">
-        <v>9645</v>
+        <v>3164</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E7" s="2">
         <v>2024</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>129</v>
+        <v>150</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>155</v>
+        <v>179</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>177</v>
+        <v>203</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>201</v>
+        <v>229</v>
       </c>
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C8" s="2">
-        <v>9645</v>
+        <v>6919</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E8" s="2">
         <v>2024</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>129</v>
+        <v>151</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>155</v>
+        <v>180</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>177</v>
+        <v>204</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>201</v>
+        <v>230</v>
       </c>
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C9" s="2">
-        <v>3164</v>
+        <v>9302</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E9" s="2">
         <v>2024</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>130</v>
+        <v>152</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>156</v>
+        <v>181</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>178</v>
+        <v>205</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>202</v>
+        <v>231</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -1472,281 +1566,273 @@
         <v>17</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C10" s="2">
-        <v>6919</v>
+        <v>828</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E10" s="2">
         <v>2024</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>17</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>131</v>
+        <v>153</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>157</v>
+        <v>182</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>179</v>
+        <v>206</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>203</v>
+        <v>232</v>
       </c>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C11" s="2">
-        <v>9302</v>
+        <v>4398</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E11" s="2">
         <v>2024</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>158</v>
+        <v>183</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>180</v>
+        <v>207</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>204</v>
+        <v>228</v>
       </c>
     </row>
     <row r="12" spans="1:15">
       <c r="A12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C12" s="2">
-        <v>828</v>
+        <v>3705</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E12" s="2">
         <v>2024</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>133</v>
+        <v>147</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>159</v>
+        <v>176</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>181</v>
+        <v>200</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>205</v>
+        <v>225</v>
       </c>
     </row>
     <row r="13" spans="1:15">
       <c r="A13" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="2">
-        <v>4398</v>
+        <v>3705</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E13" s="2">
         <v>2024</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>160</v>
+        <v>176</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>182</v>
+        <v>200</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>200</v>
+        <v>225</v>
       </c>
     </row>
     <row r="14" spans="1:15">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C14" s="2">
-        <v>3705</v>
+        <v>1983</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E14" s="2">
         <v>2024</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>174</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
       <c r="O14" s="1" t="s">
-        <v>197</v>
+        <v>233</v>
       </c>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C15" s="2">
-        <v>3705</v>
+        <v>1983</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E15" s="2">
         <v>2024</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>174</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
       <c r="O15" s="1" t="s">
-        <v>197</v>
+        <v>233</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -1757,90 +1843,86 @@
         <v>32</v>
       </c>
       <c r="C16" s="2">
-        <v>3222</v>
+        <v>8512</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E16" s="2">
         <v>2024</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>18</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>135</v>
+        <v>156</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>161</v>
+        <v>184</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>183</v>
+        <v>208</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>206</v>
+        <v>234</v>
       </c>
     </row>
     <row r="17" spans="1:15">
       <c r="A17" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C17" s="2">
-        <v>8512</v>
+        <v>1983</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E17" s="2">
         <v>2024</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>184</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
       <c r="O17" s="1" t="s">
-        <v>207</v>
+        <v>233</v>
       </c>
     </row>
     <row r="18" spans="1:15">
@@ -1851,90 +1933,90 @@
         <v>34</v>
       </c>
       <c r="C18" s="2">
-        <v>3222</v>
+        <v>8512</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E18" s="2">
         <v>2024</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>18</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>135</v>
+        <v>156</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>161</v>
+        <v>184</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>183</v>
+        <v>208</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>206</v>
+        <v>234</v>
       </c>
     </row>
     <row r="19" spans="1:15">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C19" s="2">
-        <v>7640</v>
+        <v>3222</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E19" s="2">
         <v>2024</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>137</v>
+        <v>157</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>163</v>
+        <v>185</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>185</v>
+        <v>209</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>208</v>
+        <v>235</v>
       </c>
     </row>
     <row r="20" spans="1:15">
@@ -1942,563 +2024,563 @@
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C20" s="2">
-        <v>7640</v>
+        <v>8512</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E20" s="2">
         <v>2024</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>18</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>137</v>
+        <v>156</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>163</v>
+        <v>186</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>185</v>
+        <v>210</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>208</v>
+        <v>234</v>
       </c>
     </row>
     <row r="21" spans="1:15">
       <c r="A21" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C21" s="2">
-        <v>7640</v>
+        <v>3222</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E21" s="2">
         <v>2024</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>137</v>
+        <v>157</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>163</v>
+        <v>185</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>185</v>
+        <v>209</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>208</v>
+        <v>235</v>
       </c>
     </row>
     <row r="22" spans="1:15">
       <c r="A22" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C22" s="2">
-        <v>9645</v>
+        <v>7640</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E22" s="2">
         <v>2024</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>83</v>
+        <v>101</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>155</v>
+        <v>187</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>177</v>
+        <v>211</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>201</v>
+        <v>236</v>
       </c>
     </row>
     <row r="23" spans="1:15">
       <c r="A23" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C23" s="2">
-        <v>9645</v>
+        <v>7640</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E23" s="2">
         <v>2024</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>155</v>
+        <v>187</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>177</v>
+        <v>211</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>201</v>
+        <v>236</v>
       </c>
     </row>
     <row r="24" spans="1:15">
       <c r="A24" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C24" s="2">
-        <v>2856</v>
+        <v>7640</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E24" s="2">
         <v>2024</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>139</v>
+        <v>158</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>164</v>
+        <v>187</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>186</v>
+        <v>211</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>209</v>
+        <v>236</v>
       </c>
     </row>
     <row r="25" spans="1:15">
       <c r="A25" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C25" s="2">
-        <v>2855</v>
+        <v>9624</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E25" s="2">
         <v>2024</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>139</v>
+        <v>159</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>164</v>
+        <v>188</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>186</v>
+        <v>212</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>210</v>
+        <v>237</v>
       </c>
     </row>
     <row r="26" spans="1:15">
       <c r="A26" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C26" s="2">
-        <v>3661</v>
+        <v>9624</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E26" s="2">
         <v>2024</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>140</v>
+        <v>159</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>165</v>
+        <v>188</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>187</v>
+        <v>212</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>211</v>
+        <v>237</v>
       </c>
     </row>
     <row r="27" spans="1:15">
       <c r="A27" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C27" s="2">
-        <v>6384</v>
+        <v>2855</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E27" s="2">
         <v>2024</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>141</v>
+        <v>160</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>166</v>
+        <v>189</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>188</v>
+        <v>213</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>212</v>
+        <v>238</v>
       </c>
     </row>
     <row r="28" spans="1:15">
       <c r="A28" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C28" s="2">
-        <v>5471</v>
+        <v>2856</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E28" s="2">
         <v>2024</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>142</v>
+        <v>160</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>167</v>
+        <v>189</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>213</v>
+        <v>239</v>
       </c>
     </row>
     <row r="29" spans="1:15">
       <c r="A29" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C29" s="2">
-        <v>4273</v>
+        <v>9624</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E29" s="2">
         <v>2024</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>143</v>
+        <v>159</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>167</v>
+        <v>188</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>189</v>
+        <v>212</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>214</v>
+        <v>237</v>
       </c>
     </row>
     <row r="30" spans="1:15">
       <c r="A30" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C30" s="2">
-        <v>7684</v>
+        <v>7981</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E30" s="2">
         <v>2024</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>144</v>
+        <v>161</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>168</v>
+        <v>190</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>215</v>
+        <v>240</v>
       </c>
     </row>
     <row r="31" spans="1:15">
       <c r="A31" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C31" s="2">
-        <v>9521</v>
+        <v>9301</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E31" s="2">
         <v>2024</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>145</v>
+        <v>161</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>159</v>
+        <v>190</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>181</v>
+        <v>214</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
     </row>
     <row r="32" spans="1:15">
@@ -2509,43 +2591,43 @@
         <v>43</v>
       </c>
       <c r="C32" s="2">
-        <v>9521</v>
+        <v>6384</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E32" s="2">
         <v>2024</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>17</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>146</v>
+        <v>162</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>169</v>
+        <v>191</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>216</v>
+        <v>242</v>
       </c>
     </row>
     <row r="33" spans="1:15">
@@ -2556,283 +2638,283 @@
         <v>44</v>
       </c>
       <c r="C33" s="2">
-        <v>7640</v>
+        <v>5471</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E33" s="2">
         <v>2024</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="K33" s="1" t="s">
         <v>18</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>137</v>
+        <v>163</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>163</v>
+        <v>192</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>185</v>
+        <v>216</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>208</v>
+        <v>243</v>
       </c>
     </row>
     <row r="34" spans="1:15">
       <c r="A34" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C34" s="2">
-        <v>9645</v>
+        <v>4273</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E34" s="2">
         <v>2024</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>155</v>
+        <v>192</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>177</v>
+        <v>216</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>201</v>
+        <v>244</v>
       </c>
     </row>
     <row r="35" spans="1:15">
       <c r="A35" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C35" s="2">
-        <v>8740</v>
+        <v>7684</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E35" s="2">
         <v>2024</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>147</v>
+        <v>165</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>152</v>
+        <v>193</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>174</v>
+        <v>217</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>217</v>
+        <v>245</v>
       </c>
     </row>
     <row r="36" spans="1:15">
       <c r="A36" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C36" s="2">
-        <v>4711</v>
+        <v>9521</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E36" s="2">
         <v>2024</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>148</v>
+        <v>166</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>170</v>
+        <v>182</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>192</v>
+        <v>206</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>218</v>
+        <v>246</v>
       </c>
     </row>
     <row r="37" spans="1:15">
       <c r="A37" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C37" s="2">
-        <v>9281</v>
+        <v>9521</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E37" s="2">
         <v>2024</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>149</v>
+        <v>167</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>171</v>
+        <v>194</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>193</v>
+        <v>218</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>219</v>
+        <v>246</v>
       </c>
     </row>
     <row r="38" spans="1:15">
       <c r="A38" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C38" s="2">
-        <v>8512</v>
+        <v>9624</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E38" s="2">
         <v>2024</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>136</v>
+        <v>168</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>162</v>
+        <v>195</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>184</v>
+        <v>219</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>207</v>
+        <v>237</v>
       </c>
     </row>
     <row r="39" spans="1:15">
       <c r="A39" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>50</v>
@@ -2841,87 +2923,553 @@
         <v>7640</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E39" s="2">
         <v>2024</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>172</v>
+        <v>187</v>
       </c>
       <c r="N39" s="1" t="s">
-        <v>194</v>
+        <v>211</v>
       </c>
       <c r="O39" s="1" t="s">
-        <v>208</v>
+        <v>236</v>
       </c>
     </row>
     <row r="40" spans="1:15">
       <c r="A40" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C40" s="2">
+        <v>9624</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E40" s="2">
+        <v>2024</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="N40" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="O40" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15">
+      <c r="A41" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C41" s="2">
+        <v>8740</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E41" s="2">
+        <v>2024</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="O41" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15">
+      <c r="A42" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C42" s="2">
+        <v>4711</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E42" s="2">
+        <v>2024</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="N42" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="O42" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15">
+      <c r="A43" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C43" s="2">
+        <v>9281</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E43" s="2">
+        <v>2024</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="M43" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="N43" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="O43" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15">
+      <c r="A44" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C44" s="2">
+        <v>3705</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E44" s="2">
+        <v>2024</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="M44" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="N44" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="O44" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15">
+      <c r="A45" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C45" s="2">
+        <v>8317</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E45" s="2">
+        <v>2024</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="M45" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="N45" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="O45" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15">
+      <c r="A46" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C46" s="2">
+        <v>1983</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E46" s="2">
+        <v>2024</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="M46" s="1"/>
+      <c r="N46" s="1"/>
+      <c r="O46" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15">
+      <c r="A47" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C47" s="2">
+        <v>3705</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E47" s="2">
+        <v>2024</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L47" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="M47" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="N47" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="O47" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15">
+      <c r="A48" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C48" s="2">
+        <v>8512</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E48" s="2">
+        <v>2024</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="M48" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="N48" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="O48" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15">
+      <c r="A49" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C49" s="2">
+        <v>7640</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E49" s="2">
+        <v>2024</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L49" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="M49" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="N49" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="O49" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15">
+      <c r="A50" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C50" s="2">
         <v>3553</v>
       </c>
-      <c r="D40" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E40" s="2">
-        <v>2024</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="I40" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="J40" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="K40" s="1" t="s">
+      <c r="D50" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E50" s="2">
+        <v>2024</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="K50" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L40" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="M40" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="N40" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="O40" s="1" t="s">
-        <v>220</v>
+      <c r="L50" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="M50" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="N50" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="O50" s="1" t="s">
+        <v>251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>